<commit_message>
plotted pool testing and negated depth error
</commit_message>
<xml_diff>
--- a/logging/16-07-28 good mission results.xlsx
+++ b/logging/16-07-28 good mission results.xlsx
@@ -167,15 +167,1474 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>16-07-29</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Successful Mission (Kc=9.6, Ti=1.6, Td=14.1)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Set Depth</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$J:$J</c:f>
+              <c:strCache>
+                <c:ptCount val="227"/>
+                <c:pt idx="1">
+                  <c:v>time</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17.25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18.25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19.25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20.25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>23.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>24.25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>25.25</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>26.25</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>27.25</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>28.25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>29.25</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>30.25</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>31.25</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>32.25</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>33.3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>34.3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>35.3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>36.3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>37.3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>38.3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>39.3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>40.3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>41.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42.35</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43.35</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>44.35</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>45.35</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>46.35</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>47.35</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>48.35</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>49.35</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>50.35</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>51.35</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>52.35</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>53.35</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>54.35</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>55.35</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>56.35</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>57.35</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>58.35</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>59.4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>60.4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>62.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>63.4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>64.4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>65.4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>66.4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>67.4</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>68.4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>69.4</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>70.4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>71.4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>72.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>73.4</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>74.45</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>75.45</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>76.45</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>77.45</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>78.45</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>79.45</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>80.45</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>81.45</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>82.45</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>83.45</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>84.5</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>85.5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>87.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>88.5</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>89.5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>90.5</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>91.5</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>93.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>94.5</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>98.5</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>99.5</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>100.5</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>101.55</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>102.55</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>103.55</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>104.55</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>105.55</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>106.55</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>107.55</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>108.55</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>109.55</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>110.55</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>111.55</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>112.55</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>113.55</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>114.55</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>115.55</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>116.55</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>117.6</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>118.6</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>119.6</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>120.6</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>121.6</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>122.6</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>123.6</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>124.6</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>125.6</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>126.65</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>127.65</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>128.65</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>129.65</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>130.65</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>131.65</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>132.65</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>133.65</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>134.65</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>135.65</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>136.65</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>137.65</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>138.65</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>139.65</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>140.65</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>141.65</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>142.7</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>143.7</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>144.7</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>145.7</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>146.7</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>147.7</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>148.7</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>149.7</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>150.7</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>151.7</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>152.7</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>153.7</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>154.7</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>155.7</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>156.7</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>157.71</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>158.76</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>159.76</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>160.76</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>161.76</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>162.76</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>163.76</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>164.76</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>165.76</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>166.76</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>167.81</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>168.81</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>169.81</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>170.81</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>171.81</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>172.81</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>173.81</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>174.81</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>175.81</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>176.81</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>177.81</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>178.81</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>179.81</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>180.81</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>181.81</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>182.81</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>183.81</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>184.86</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>185.86</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>186.86</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>187.86</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>188.86</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>189.86</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>190.86</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>191.86</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>192.86</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>193.86</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>194.86</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>195.86</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>196.86</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>197.86</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>198.86</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>199.91</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>200.91</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>201.91</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>202.91</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>203.91</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>204.91</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>205.11</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>205.11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E:$E</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8C65-4461-8CEC-3C4260008456}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>BCU Depth</c:v>
           </c:tx>
@@ -1573,7 +3032,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>BCU Depth Error</c:v>
           </c:tx>
@@ -2285,679 +3744,679 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46639999999999998</c:v>
+                  <c:v>-0.46639999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42970000000000003</c:v>
+                  <c:v>-0.42970000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.37669999999999998</c:v>
+                  <c:v>-0.37669999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.30930000000000002</c:v>
+                  <c:v>-0.30930000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29399999999999998</c:v>
+                  <c:v>-0.29399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2797</c:v>
+                  <c:v>-0.2797</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.29099999999999998</c:v>
+                  <c:v>-0.29099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2767</c:v>
+                  <c:v>-0.2767</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2777</c:v>
+                  <c:v>-0.2777</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2389</c:v>
+                  <c:v>-0.2389</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.20219999999999999</c:v>
+                  <c:v>-0.20219999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1573</c:v>
+                  <c:v>-0.1573</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.11849999999999999</c:v>
+                  <c:v>-0.11849999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.0599999999999996E-2</c:v>
+                  <c:v>-7.0599999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.3E-3</c:v>
+                  <c:v>-4.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-4.3700000000000003E-2</c:v>
+                  <c:v>4.3700000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.1028</c:v>
+                  <c:v>0.1028</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.14360000000000001</c:v>
+                  <c:v>0.14360000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.16300000000000001</c:v>
+                  <c:v>0.16300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.1181</c:v>
+                  <c:v>0.1181</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-5.0799999999999998E-2</c:v>
+                  <c:v>5.0799999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.47E-2</c:v>
+                  <c:v>-2.47E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.0999999999999998E-2</c:v>
+                  <c:v>-9.0999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.13900000000000001</c:v>
+                  <c:v>-0.13900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.14610000000000001</c:v>
+                  <c:v>-0.14610000000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.13589999999999999</c:v>
+                  <c:v>-0.13589999999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.1226</c:v>
+                  <c:v>-0.1226</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.10630000000000001</c:v>
+                  <c:v>-0.10630000000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.5700000000000003E-2</c:v>
+                  <c:v>-7.5700000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.7999999999999999E-2</c:v>
+                  <c:v>-3.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-1.61E-2</c:v>
+                  <c:v>1.61E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-5.6899999999999999E-2</c:v>
+                  <c:v>5.6899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-0.1018</c:v>
+                  <c:v>0.1018</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-0.1263</c:v>
+                  <c:v>0.1263</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.1222</c:v>
+                  <c:v>0.1222</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-8.5500000000000007E-2</c:v>
+                  <c:v>8.5500000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-2.63E-2</c:v>
+                  <c:v>2.63E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.39E-2</c:v>
+                  <c:v>-3.39E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.0799999999999997E-2</c:v>
+                  <c:v>-8.0799999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.1053</c:v>
+                  <c:v>-0.1053</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.1145</c:v>
+                  <c:v>-0.1145</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.1114</c:v>
+                  <c:v>-0.1114</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>9.7100000000000006E-2</c:v>
+                  <c:v>-9.7100000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.0613999999999999</c:v>
+                  <c:v>-1.0613999999999999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.0348999999999999</c:v>
+                  <c:v>-1.0348999999999999</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.99199999999999999</c:v>
+                  <c:v>-0.99199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.95120000000000005</c:v>
+                  <c:v>-0.95120000000000005</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.8972</c:v>
+                  <c:v>-0.8972</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.84109999999999996</c:v>
+                  <c:v>-0.84109999999999996</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.77170000000000005</c:v>
+                  <c:v>-0.77170000000000005</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.70130000000000003</c:v>
+                  <c:v>-0.70130000000000003</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.62890000000000001</c:v>
+                  <c:v>-0.62890000000000001</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.5625</c:v>
+                  <c:v>-0.5625</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.47889999999999999</c:v>
+                  <c:v>-0.47889999999999999</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.40129999999999999</c:v>
+                  <c:v>-0.40129999999999999</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.3075</c:v>
+                  <c:v>-0.3075</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.2157</c:v>
+                  <c:v>-0.2157</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.1157</c:v>
+                  <c:v>-0.1157</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>8.6E-3</c:v>
+                  <c:v>-8.6E-3</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-9.4500000000000001E-2</c:v>
+                  <c:v>9.4500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-0.1842</c:v>
+                  <c:v>0.1842</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-0.25869999999999999</c:v>
+                  <c:v>0.25869999999999999</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-0.27810000000000001</c:v>
+                  <c:v>0.27810000000000001</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>-0.2495</c:v>
+                  <c:v>0.2495</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-0.19850000000000001</c:v>
+                  <c:v>0.19850000000000001</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>-0.11899999999999999</c:v>
+                  <c:v>0.11899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-3.5299999999999998E-2</c:v>
+                  <c:v>3.5299999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>-3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>6.0600000000000001E-2</c:v>
+                  <c:v>-6.0600000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.1400000000000001E-2</c:v>
+                  <c:v>-5.1400000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-5.9999999999999995E-4</c:v>
+                  <c:v>5.9999999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>-7.7100000000000002E-2</c:v>
+                  <c:v>7.7100000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>-0.1424</c:v>
+                  <c:v>0.1424</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>-0.1822</c:v>
+                  <c:v>0.1822</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>-0.19650000000000001</c:v>
+                  <c:v>0.19650000000000001</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-0.16689999999999999</c:v>
+                  <c:v>0.16689999999999999</c:v>
                 </c:pt>
                 <c:pt idx="77">
+                  <c:v>9.9599999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.29E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-5.2400000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-9.0200000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-9.2200000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-4.8399999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.41E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.7300000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-0.87080000000000002</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-0.84640000000000004</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-0.8004</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-0.69430000000000003</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-0.57499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-0.4536</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-0.31690000000000002</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-0.19239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.3099999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.1351</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.1993</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.22889999999999999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.22589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.184</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.1167</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>6.1600000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-7.7999999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-6.2799999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-6.08E-2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>4.1200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.1096</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.16159999999999999</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.18509999999999999</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.1769</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.14319999999999999</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.9800000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>-5.0599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>-9.35E-2</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>-9.9599999999999994E-2</c:v>
                 </c:pt>
-                <c:pt idx="78">
-                  <c:v>-1.29E-2</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>5.2400000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>9.0200000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>9.2200000000000004E-2</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>4.8399999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>-2.41E-2</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>-8.7300000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.87080000000000002</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.84640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.8004</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.69430000000000003</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.57499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.4536</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.31690000000000002</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.19239999999999999</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>-3.3099999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>-0.1351</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>-0.1993</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>-0.22889999999999999</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>-0.23</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>-0.22589999999999999</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>-0.184</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>-0.1167</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>-6.1600000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>7.7999999999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>6.2799999999999995E-2</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>6.08E-2</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>2.1999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>-4.1200000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>-0.1096</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>-0.16159999999999999</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>-0.18509999999999999</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>-0.1769</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>-0.14319999999999999</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>-0.08</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>-1.9800000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>5.0599999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>9.35E-2</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>9.9599999999999994E-2</c:v>
-                </c:pt>
                 <c:pt idx="118">
-                  <c:v>3.6299999999999999E-2</c:v>
+                  <c:v>-3.6299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>-2.9000000000000001E-2</c:v>
+                  <c:v>2.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>-9.6299999999999997E-2</c:v>
+                  <c:v>9.6299999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>0.34250000000000003</c:v>
+                  <c:v>-0.34250000000000003</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>0.26190000000000002</c:v>
+                  <c:v>-0.26190000000000002</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>0.15479999999999999</c:v>
+                  <c:v>-0.15479999999999999</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2.8299999999999999E-2</c:v>
+                  <c:v>-2.8299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>-9.6199999999999994E-2</c:v>
+                  <c:v>9.6199999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>-0.20230000000000001</c:v>
+                  <c:v>0.20230000000000001</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>-0.2747</c:v>
+                  <c:v>0.2747</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>-0.33600000000000002</c:v>
+                  <c:v>0.33600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>-0.32879999999999998</c:v>
+                  <c:v>0.32879999999999998</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>-0.32979999999999998</c:v>
+                  <c:v>0.32979999999999998</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>-0.30940000000000001</c:v>
+                  <c:v>0.30940000000000001</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>-0.29409999999999997</c:v>
+                  <c:v>0.29409999999999997</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>-0.26150000000000001</c:v>
+                  <c:v>0.26150000000000001</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>-0.24210000000000001</c:v>
+                  <c:v>0.24210000000000001</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>-0.19719999999999999</c:v>
+                  <c:v>0.19719999999999999</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>-0.16969999999999999</c:v>
+                  <c:v>0.16969999999999999</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>-0.14419999999999999</c:v>
+                  <c:v>0.14419999999999999</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>-0.11459999999999999</c:v>
+                  <c:v>0.11459999999999999</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>-7.2700000000000001E-2</c:v>
+                  <c:v>7.2700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>-4.2099999999999999E-2</c:v>
+                  <c:v>4.2099999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>-4.4000000000000003E-3</c:v>
+                  <c:v>4.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>2.4199999999999999E-2</c:v>
+                  <c:v>-2.4199999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>4.2500000000000003E-2</c:v>
+                  <c:v>-4.2500000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>3.7400000000000003E-2</c:v>
+                  <c:v>-3.7400000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>3.8E-3</c:v>
+                  <c:v>-3.8E-3</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>-1.0523</c:v>
+                  <c:v>1.0523</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>-1.1073999999999999</c:v>
+                  <c:v>1.1073999999999999</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>-1.1554</c:v>
+                  <c:v>1.1554</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>-1.1879999999999999</c:v>
+                  <c:v>1.1879999999999999</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>-1.2042999999999999</c:v>
+                  <c:v>1.2042999999999999</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>-1.2185999999999999</c:v>
+                  <c:v>1.2185999999999999</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>-1.2144999999999999</c:v>
+                  <c:v>1.2144999999999999</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>-1.2124999999999999</c:v>
+                  <c:v>1.2124999999999999</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>-1.2022999999999999</c:v>
+                  <c:v>1.2022999999999999</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>-1.1850000000000001</c:v>
+                  <c:v>1.1850000000000001</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>-1.1625000000000001</c:v>
+                  <c:v>1.1625000000000001</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>-1.1391</c:v>
+                  <c:v>1.1391</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>-1.1053999999999999</c:v>
+                  <c:v>1.1053999999999999</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>-1.0809</c:v>
+                  <c:v>1.0809</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>-1.0421</c:v>
+                  <c:v>1.0421</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>-1.0054000000000001</c:v>
+                  <c:v>1.0054000000000001</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>-0.9738</c:v>
+                  <c:v>0.9738</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>-0.92579999999999996</c:v>
+                  <c:v>0.92579999999999996</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>-0.88400000000000001</c:v>
+                  <c:v>0.88400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>-0.84630000000000005</c:v>
+                  <c:v>0.84630000000000005</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>-0.79930000000000001</c:v>
+                  <c:v>0.79930000000000001</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>-0.74929999999999997</c:v>
+                  <c:v>0.74929999999999997</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>-0.70240000000000002</c:v>
+                  <c:v>0.70240000000000002</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>-0.64529999999999998</c:v>
+                  <c:v>0.64529999999999998</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>-0.59530000000000005</c:v>
+                  <c:v>0.59530000000000005</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>-0.54530000000000001</c:v>
+                  <c:v>0.54530000000000001</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>-0.48509999999999998</c:v>
+                  <c:v>0.48509999999999998</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>-0.43309999999999998</c:v>
+                  <c:v>0.43309999999999998</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>-0.3861</c:v>
+                  <c:v>0.3861</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>-0.32600000000000001</c:v>
+                  <c:v>0.32600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>-0.26369999999999999</c:v>
+                  <c:v>0.26369999999999999</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>-0.2097</c:v>
+                  <c:v>0.2097</c:v>
                 </c:pt>
                 <c:pt idx="178">
+                  <c:v>0.13819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>7.6999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1.4800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>-5.1499999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>-0.1178</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>-0.1709</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>-0.18820000000000001</c:v>
+                </c:pt>
+                <c:pt idx="185">
                   <c:v>-0.13819999999999999</c:v>
                 </c:pt>
-                <c:pt idx="179">
-                  <c:v>-7.6999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>-1.4800000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>5.1499999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>0.1178</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>0.1709</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>0.18820000000000001</c:v>
-                </c:pt>
-                <c:pt idx="185">
+                <c:pt idx="186">
+                  <c:v>-7.2900000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>1.17E-2</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>8.72E-2</c:v>
+                </c:pt>
+                <c:pt idx="189">
                   <c:v>0.13819999999999999</c:v>
                 </c:pt>
-                <c:pt idx="186">
-                  <c:v>7.2900000000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>-1.17E-2</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>-8.72E-2</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>-0.13819999999999999</c:v>
-                </c:pt>
                 <c:pt idx="190">
-                  <c:v>-0.16070000000000001</c:v>
+                  <c:v>0.16070000000000001</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>-0.1515</c:v>
+                  <c:v>0.1515</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>-0.1138</c:v>
+                  <c:v>0.1138</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>-4.7399999999999998E-2</c:v>
+                  <c:v>4.7399999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>3.0099999999999998E-2</c:v>
+                  <c:v>-3.0099999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>0.10150000000000001</c:v>
+                  <c:v>-0.10150000000000001</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>0.125</c:v>
+                  <c:v>-0.125</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>0.1046</c:v>
+                  <c:v>-0.1046</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>5.6599999999999998E-2</c:v>
+                  <c:v>-5.6599999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>-2.3E-2</c:v>
+                  <c:v>2.3E-2</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>-9.8400000000000001E-2</c:v>
+                  <c:v>9.8400000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>-0.1474</c:v>
+                  <c:v>0.1474</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>-0.1699</c:v>
+                  <c:v>0.1699</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>-0.1484</c:v>
+                  <c:v>0.1484</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>-0.1138</c:v>
+                  <c:v>0.1138</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>-4.1300000000000003E-2</c:v>
+                  <c:v>4.1300000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>-2.4607000000000001</c:v>
+                  <c:v>2.4607000000000001</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>-2.3607</c:v>
+                  <c:v>2.3607</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>-2.2566999999999999</c:v>
+                  <c:v>2.2566999999999999</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>-2.1475</c:v>
+                  <c:v>2.1475</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>-2.0434999999999999</c:v>
+                  <c:v>2.0434999999999999</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>-1.9322999999999999</c:v>
+                  <c:v>1.9322999999999999</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>-1.8262</c:v>
+                  <c:v>1.8262</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>-1.7262</c:v>
+                  <c:v>1.7262</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>-1.6242000000000001</c:v>
+                  <c:v>1.6242000000000001</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>-1.5344</c:v>
+                  <c:v>1.5344</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>-1.4323999999999999</c:v>
+                  <c:v>1.4323999999999999</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>-1.3324</c:v>
+                  <c:v>1.3324</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>-1.2181</c:v>
+                  <c:v>1.2181</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>-1.1212</c:v>
+                  <c:v>1.1212</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>-1.0109999999999999</c:v>
+                  <c:v>1.0109999999999999</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>-0.89980000000000004</c:v>
+                  <c:v>0.89980000000000004</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>-0.79579999999999995</c:v>
+                  <c:v>0.79579999999999995</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>-0.6764</c:v>
+                  <c:v>0.6764</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>-0.57230000000000003</c:v>
+                  <c:v>0.57230000000000003</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>-0.44579999999999997</c:v>
+                  <c:v>0.44579999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2971,7 +4430,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>Actuator1 Pos</c:v>
           </c:tx>
@@ -4369,7 +5828,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:v>Actuator2 Pos</c:v>
           </c:tx>
@@ -6676,16 +8135,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6977,7 +8436,7 @@
   <dimension ref="A1:L227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7059,7 +8518,7 @@
         <v>0.53</v>
       </c>
       <c r="I3">
-        <v>0.46639999999999998</v>
+        <v>-0.46639999999999998</v>
       </c>
       <c r="J3">
         <v>0.2</v>
@@ -7097,7 +8556,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="I4">
-        <v>0.42970000000000003</v>
+        <v>-0.42970000000000003</v>
       </c>
       <c r="J4">
         <v>1.2</v>
@@ -7135,7 +8594,7 @@
         <v>0.62</v>
       </c>
       <c r="I5">
-        <v>0.37669999999999998</v>
+        <v>-0.37669999999999998</v>
       </c>
       <c r="J5">
         <v>2.2000000000000002</v>
@@ -7173,7 +8632,7 @@
         <v>0.69</v>
       </c>
       <c r="I6">
-        <v>0.30930000000000002</v>
+        <v>-0.30930000000000002</v>
       </c>
       <c r="J6">
         <v>3.2</v>
@@ -7211,7 +8670,7 @@
         <v>0.71</v>
       </c>
       <c r="I7">
-        <v>0.29399999999999998</v>
+        <v>-0.29399999999999998</v>
       </c>
       <c r="J7">
         <v>4.2</v>
@@ -7249,7 +8708,7 @@
         <v>0.72</v>
       </c>
       <c r="I8">
-        <v>0.2797</v>
+        <v>-0.2797</v>
       </c>
       <c r="J8">
         <v>5.2</v>
@@ -7287,7 +8746,7 @@
         <v>0.71</v>
       </c>
       <c r="I9">
-        <v>0.29099999999999998</v>
+        <v>-0.29099999999999998</v>
       </c>
       <c r="J9">
         <v>6.2</v>
@@ -7325,7 +8784,7 @@
         <v>0.72</v>
       </c>
       <c r="I10">
-        <v>0.2767</v>
+        <v>-0.2767</v>
       </c>
       <c r="J10">
         <v>7.2</v>
@@ -7363,7 +8822,7 @@
         <v>0.72</v>
       </c>
       <c r="I11">
-        <v>0.2777</v>
+        <v>-0.2777</v>
       </c>
       <c r="J11">
         <v>8.1999999999999993</v>
@@ -7401,7 +8860,7 @@
         <v>0.76</v>
       </c>
       <c r="I12">
-        <v>0.2389</v>
+        <v>-0.2389</v>
       </c>
       <c r="J12">
         <v>9.1999999999999993</v>
@@ -7439,7 +8898,7 @@
         <v>0.8</v>
       </c>
       <c r="I13">
-        <v>0.20219999999999999</v>
+        <v>-0.20219999999999999</v>
       </c>
       <c r="J13">
         <v>10.199999999999999</v>
@@ -7477,7 +8936,7 @@
         <v>0.84</v>
       </c>
       <c r="I14">
-        <v>0.1573</v>
+        <v>-0.1573</v>
       </c>
       <c r="J14">
         <v>11.2</v>
@@ -7515,7 +8974,7 @@
         <v>0.88</v>
       </c>
       <c r="I15">
-        <v>0.11849999999999999</v>
+        <v>-0.11849999999999999</v>
       </c>
       <c r="J15">
         <v>12.2</v>
@@ -7553,7 +9012,7 @@
         <v>0.93</v>
       </c>
       <c r="I16">
-        <v>7.0599999999999996E-2</v>
+        <v>-7.0599999999999996E-2</v>
       </c>
       <c r="J16">
         <v>13.2</v>
@@ -7591,7 +9050,7 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <v>4.3E-3</v>
+        <v>-4.3E-3</v>
       </c>
       <c r="J17">
         <v>14.2</v>
@@ -7629,7 +9088,7 @@
         <v>1.04</v>
       </c>
       <c r="I18">
-        <v>-4.3700000000000003E-2</v>
+        <v>4.3700000000000003E-2</v>
       </c>
       <c r="J18">
         <v>15.2</v>
@@ -7667,7 +9126,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I19">
-        <v>-0.1028</v>
+        <v>0.1028</v>
       </c>
       <c r="J19">
         <v>16.2</v>
@@ -7705,7 +9164,7 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="I20">
-        <v>-0.14360000000000001</v>
+        <v>0.14360000000000001</v>
       </c>
       <c r="J20">
         <v>17.25</v>
@@ -7743,7 +9202,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="I21">
-        <v>-0.16300000000000001</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="J21">
         <v>18.25</v>
@@ -7781,7 +9240,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="I22">
-        <v>-0.1181</v>
+        <v>0.1181</v>
       </c>
       <c r="J22">
         <v>19.25</v>
@@ -7819,7 +9278,7 @@
         <v>1.05</v>
       </c>
       <c r="I23">
-        <v>-5.0799999999999998E-2</v>
+        <v>5.0799999999999998E-2</v>
       </c>
       <c r="J23">
         <v>20.25</v>
@@ -7857,7 +9316,7 @@
         <v>0.98</v>
       </c>
       <c r="I24">
-        <v>2.47E-2</v>
+        <v>-2.47E-2</v>
       </c>
       <c r="J24">
         <v>21.25</v>
@@ -7895,7 +9354,7 @@
         <v>0.91</v>
       </c>
       <c r="I25">
-        <v>9.0999999999999998E-2</v>
+        <v>-9.0999999999999998E-2</v>
       </c>
       <c r="J25">
         <v>22.25</v>
@@ -7933,7 +9392,7 @@
         <v>0.86</v>
       </c>
       <c r="I26">
-        <v>0.13900000000000001</v>
+        <v>-0.13900000000000001</v>
       </c>
       <c r="J26">
         <v>23.25</v>
@@ -7971,7 +9430,7 @@
         <v>0.85</v>
       </c>
       <c r="I27">
-        <v>0.14610000000000001</v>
+        <v>-0.14610000000000001</v>
       </c>
       <c r="J27">
         <v>24.25</v>
@@ -8009,7 +9468,7 @@
         <v>0.86</v>
       </c>
       <c r="I28">
-        <v>0.13589999999999999</v>
+        <v>-0.13589999999999999</v>
       </c>
       <c r="J28">
         <v>25.25</v>
@@ -8047,7 +9506,7 @@
         <v>0.88</v>
       </c>
       <c r="I29">
-        <v>0.1226</v>
+        <v>-0.1226</v>
       </c>
       <c r="J29">
         <v>26.25</v>
@@ -8085,7 +9544,7 @@
         <v>0.89</v>
       </c>
       <c r="I30">
-        <v>0.10630000000000001</v>
+        <v>-0.10630000000000001</v>
       </c>
       <c r="J30">
         <v>27.25</v>
@@ -8123,7 +9582,7 @@
         <v>0.92</v>
       </c>
       <c r="I31">
-        <v>7.5700000000000003E-2</v>
+        <v>-7.5700000000000003E-2</v>
       </c>
       <c r="J31">
         <v>28.25</v>
@@ -8161,7 +9620,7 @@
         <v>0.96</v>
       </c>
       <c r="I32">
-        <v>3.7999999999999999E-2</v>
+        <v>-3.7999999999999999E-2</v>
       </c>
       <c r="J32">
         <v>29.25</v>
@@ -8199,7 +9658,7 @@
         <v>1.02</v>
       </c>
       <c r="I33">
-        <v>-1.61E-2</v>
+        <v>1.61E-2</v>
       </c>
       <c r="J33">
         <v>30.25</v>
@@ -8237,7 +9696,7 @@
         <v>1.06</v>
       </c>
       <c r="I34">
-        <v>-5.6899999999999999E-2</v>
+        <v>5.6899999999999999E-2</v>
       </c>
       <c r="J34">
         <v>31.25</v>
@@ -8275,7 +9734,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I35">
-        <v>-0.1018</v>
+        <v>0.1018</v>
       </c>
       <c r="J35">
         <v>32.25</v>
@@ -8313,7 +9772,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="I36">
-        <v>-0.1263</v>
+        <v>0.1263</v>
       </c>
       <c r="J36">
         <v>33.299999999999997</v>
@@ -8351,7 +9810,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="I37">
-        <v>-0.1222</v>
+        <v>0.1222</v>
       </c>
       <c r="J37">
         <v>34.299999999999997</v>
@@ -8389,7 +9848,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="I38">
-        <v>-8.5500000000000007E-2</v>
+        <v>8.5500000000000007E-2</v>
       </c>
       <c r="J38">
         <v>35.299999999999997</v>
@@ -8427,7 +9886,7 @@
         <v>1.03</v>
       </c>
       <c r="I39">
-        <v>-2.63E-2</v>
+        <v>2.63E-2</v>
       </c>
       <c r="J39">
         <v>36.299999999999997</v>
@@ -8465,7 +9924,7 @@
         <v>0.97</v>
       </c>
       <c r="I40">
-        <v>3.39E-2</v>
+        <v>-3.39E-2</v>
       </c>
       <c r="J40">
         <v>37.299999999999997</v>
@@ -8503,7 +9962,7 @@
         <v>0.92</v>
       </c>
       <c r="I41">
-        <v>8.0799999999999997E-2</v>
+        <v>-8.0799999999999997E-2</v>
       </c>
       <c r="J41">
         <v>38.299999999999997</v>
@@ -8541,7 +10000,7 @@
         <v>0.89</v>
       </c>
       <c r="I42">
-        <v>0.1053</v>
+        <v>-0.1053</v>
       </c>
       <c r="J42">
         <v>39.299999999999997</v>
@@ -8579,7 +10038,7 @@
         <v>0.89</v>
       </c>
       <c r="I43">
-        <v>0.1145</v>
+        <v>-0.1145</v>
       </c>
       <c r="J43">
         <v>40.299999999999997</v>
@@ -8617,7 +10076,7 @@
         <v>0.89</v>
       </c>
       <c r="I44">
-        <v>0.1114</v>
+        <v>-0.1114</v>
       </c>
       <c r="J44">
         <v>41.3</v>
@@ -8655,7 +10114,7 @@
         <v>0.9</v>
       </c>
       <c r="I45">
-        <v>9.7100000000000006E-2</v>
+        <v>-9.7100000000000006E-2</v>
       </c>
       <c r="J45">
         <v>42.35</v>
@@ -8693,7 +10152,7 @@
         <v>0.94</v>
       </c>
       <c r="I46">
-        <v>1.0613999999999999</v>
+        <v>-1.0613999999999999</v>
       </c>
       <c r="J46">
         <v>43.35</v>
@@ -8731,7 +10190,7 @@
         <v>0.97</v>
       </c>
       <c r="I47">
-        <v>1.0348999999999999</v>
+        <v>-1.0348999999999999</v>
       </c>
       <c r="J47">
         <v>44.35</v>
@@ -8769,7 +10228,7 @@
         <v>1.01</v>
       </c>
       <c r="I48">
-        <v>0.99199999999999999</v>
+        <v>-0.99199999999999999</v>
       </c>
       <c r="J48">
         <v>45.35</v>
@@ -8807,7 +10266,7 @@
         <v>1.05</v>
       </c>
       <c r="I49">
-        <v>0.95120000000000005</v>
+        <v>-0.95120000000000005</v>
       </c>
       <c r="J49">
         <v>46.35</v>
@@ -8845,7 +10304,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I50">
-        <v>0.8972</v>
+        <v>-0.8972</v>
       </c>
       <c r="J50">
         <v>47.35</v>
@@ -8883,7 +10342,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="I51">
-        <v>0.84109999999999996</v>
+        <v>-0.84109999999999996</v>
       </c>
       <c r="J51">
         <v>48.35</v>
@@ -8921,7 +10380,7 @@
         <v>1.23</v>
       </c>
       <c r="I52">
-        <v>0.77170000000000005</v>
+        <v>-0.77170000000000005</v>
       </c>
       <c r="J52">
         <v>49.35</v>
@@ -8959,7 +10418,7 @@
         <v>1.3</v>
       </c>
       <c r="I53">
-        <v>0.70130000000000003</v>
+        <v>-0.70130000000000003</v>
       </c>
       <c r="J53">
         <v>50.35</v>
@@ -8997,7 +10456,7 @@
         <v>1.37</v>
       </c>
       <c r="I54">
-        <v>0.62890000000000001</v>
+        <v>-0.62890000000000001</v>
       </c>
       <c r="J54">
         <v>51.35</v>
@@ -9035,7 +10494,7 @@
         <v>1.44</v>
       </c>
       <c r="I55">
-        <v>0.5625</v>
+        <v>-0.5625</v>
       </c>
       <c r="J55">
         <v>52.35</v>
@@ -9073,7 +10532,7 @@
         <v>1.52</v>
       </c>
       <c r="I56">
-        <v>0.47889999999999999</v>
+        <v>-0.47889999999999999</v>
       </c>
       <c r="J56">
         <v>53.35</v>
@@ -9111,7 +10570,7 @@
         <v>1.6</v>
       </c>
       <c r="I57">
-        <v>0.40129999999999999</v>
+        <v>-0.40129999999999999</v>
       </c>
       <c r="J57">
         <v>54.35</v>
@@ -9149,7 +10608,7 @@
         <v>1.69</v>
       </c>
       <c r="I58">
-        <v>0.3075</v>
+        <v>-0.3075</v>
       </c>
       <c r="J58">
         <v>55.35</v>
@@ -9187,7 +10646,7 @@
         <v>1.78</v>
       </c>
       <c r="I59">
-        <v>0.2157</v>
+        <v>-0.2157</v>
       </c>
       <c r="J59">
         <v>56.35</v>
@@ -9225,7 +10684,7 @@
         <v>1.88</v>
       </c>
       <c r="I60">
-        <v>0.1157</v>
+        <v>-0.1157</v>
       </c>
       <c r="J60">
         <v>57.35</v>
@@ -9263,7 +10722,7 @@
         <v>1.99</v>
       </c>
       <c r="I61">
-        <v>8.6E-3</v>
+        <v>-8.6E-3</v>
       </c>
       <c r="J61">
         <v>58.35</v>
@@ -9301,7 +10760,7 @@
         <v>2.09</v>
       </c>
       <c r="I62">
-        <v>-9.4500000000000001E-2</v>
+        <v>9.4500000000000001E-2</v>
       </c>
       <c r="J62">
         <v>59.4</v>
@@ -9339,7 +10798,7 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="I63">
-        <v>-0.1842</v>
+        <v>0.1842</v>
       </c>
       <c r="J63">
         <v>60.4</v>
@@ -9377,7 +10836,7 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="I64">
-        <v>-0.25869999999999999</v>
+        <v>0.25869999999999999</v>
       </c>
       <c r="J64">
         <v>61.4</v>
@@ -9415,7 +10874,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="I65">
-        <v>-0.27810000000000001</v>
+        <v>0.27810000000000001</v>
       </c>
       <c r="J65">
         <v>62.4</v>
@@ -9453,7 +10912,7 @@
         <v>2.25</v>
       </c>
       <c r="I66">
-        <v>-0.2495</v>
+        <v>0.2495</v>
       </c>
       <c r="J66">
         <v>63.4</v>
@@ -9491,7 +10950,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="I67">
-        <v>-0.19850000000000001</v>
+        <v>0.19850000000000001</v>
       </c>
       <c r="J67">
         <v>64.400000000000006</v>
@@ -9529,7 +10988,7 @@
         <v>2.12</v>
       </c>
       <c r="I68">
-        <v>-0.11899999999999999</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="J68">
         <v>65.400000000000006</v>
@@ -9567,7 +11026,7 @@
         <v>2.04</v>
       </c>
       <c r="I69">
-        <v>-3.5299999999999998E-2</v>
+        <v>3.5299999999999998E-2</v>
       </c>
       <c r="J69">
         <v>66.400000000000006</v>
@@ -9605,7 +11064,7 @@
         <v>1.97</v>
       </c>
       <c r="I70">
-        <v>3.1E-2</v>
+        <v>-3.1E-2</v>
       </c>
       <c r="J70">
         <v>67.400000000000006</v>
@@ -9643,7 +11102,7 @@
         <v>1.94</v>
       </c>
       <c r="I71">
-        <v>6.0600000000000001E-2</v>
+        <v>-6.0600000000000001E-2</v>
       </c>
       <c r="J71">
         <v>68.400000000000006</v>
@@ -9681,7 +11140,7 @@
         <v>1.95</v>
       </c>
       <c r="I72">
-        <v>5.1400000000000001E-2</v>
+        <v>-5.1400000000000001E-2</v>
       </c>
       <c r="J72">
         <v>69.400000000000006</v>
@@ -9719,7 +11178,7 @@
         <v>2</v>
       </c>
       <c r="I73">
-        <v>-5.9999999999999995E-4</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="J73">
         <v>70.400000000000006</v>
@@ -9757,7 +11216,7 @@
         <v>2.08</v>
       </c>
       <c r="I74">
-        <v>-7.7100000000000002E-2</v>
+        <v>7.7100000000000002E-2</v>
       </c>
       <c r="J74">
         <v>71.400000000000006</v>
@@ -9795,7 +11254,7 @@
         <v>2.14</v>
       </c>
       <c r="I75">
-        <v>-0.1424</v>
+        <v>0.1424</v>
       </c>
       <c r="J75">
         <v>72.400000000000006</v>
@@ -9833,7 +11292,7 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="I76">
-        <v>-0.1822</v>
+        <v>0.1822</v>
       </c>
       <c r="J76">
         <v>73.400000000000006</v>
@@ -9871,7 +11330,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="I77">
-        <v>-0.19650000000000001</v>
+        <v>0.19650000000000001</v>
       </c>
       <c r="J77">
         <v>74.45</v>
@@ -9909,7 +11368,7 @@
         <v>2.17</v>
       </c>
       <c r="I78">
-        <v>-0.16689999999999999</v>
+        <v>0.16689999999999999</v>
       </c>
       <c r="J78">
         <v>75.45</v>
@@ -9947,7 +11406,7 @@
         <v>2.1</v>
       </c>
       <c r="I79">
-        <v>-9.9599999999999994E-2</v>
+        <v>9.9599999999999994E-2</v>
       </c>
       <c r="J79">
         <v>76.45</v>
@@ -9985,7 +11444,7 @@
         <v>2.0099999999999998</v>
       </c>
       <c r="I80">
-        <v>-1.29E-2</v>
+        <v>1.29E-2</v>
       </c>
       <c r="J80">
         <v>77.45</v>
@@ -10023,7 +11482,7 @@
         <v>1.95</v>
       </c>
       <c r="I81">
-        <v>5.2400000000000002E-2</v>
+        <v>-5.2400000000000002E-2</v>
       </c>
       <c r="J81">
         <v>78.45</v>
@@ -10061,7 +11520,7 @@
         <v>1.91</v>
       </c>
       <c r="I82">
-        <v>9.0200000000000002E-2</v>
+        <v>-9.0200000000000002E-2</v>
       </c>
       <c r="J82">
         <v>79.45</v>
@@ -10099,7 +11558,7 @@
         <v>1.91</v>
       </c>
       <c r="I83">
-        <v>9.2200000000000004E-2</v>
+        <v>-9.2200000000000004E-2</v>
       </c>
       <c r="J83">
         <v>80.45</v>
@@ -10137,7 +11596,7 @@
         <v>1.95</v>
       </c>
       <c r="I84">
-        <v>4.8399999999999999E-2</v>
+        <v>-4.8399999999999999E-2</v>
       </c>
       <c r="J84">
         <v>81.45</v>
@@ -10175,7 +11634,7 @@
         <v>2.02</v>
       </c>
       <c r="I85">
-        <v>-2.41E-2</v>
+        <v>2.41E-2</v>
       </c>
       <c r="J85">
         <v>82.45</v>
@@ -10213,7 +11672,7 @@
         <v>2.09</v>
       </c>
       <c r="I86">
-        <v>-8.7300000000000003E-2</v>
+        <v>8.7300000000000003E-2</v>
       </c>
       <c r="J86">
         <v>83.45</v>
@@ -10251,7 +11710,7 @@
         <v>2.13</v>
       </c>
       <c r="I87">
-        <v>0.87080000000000002</v>
+        <v>-0.87080000000000002</v>
       </c>
       <c r="J87">
         <v>84.5</v>
@@ -10289,7 +11748,7 @@
         <v>2.15</v>
       </c>
       <c r="I88">
-        <v>0.84640000000000004</v>
+        <v>-0.84640000000000004</v>
       </c>
       <c r="J88">
         <v>85.5</v>
@@ -10327,7 +11786,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="I89">
-        <v>0.8004</v>
+        <v>-0.8004</v>
       </c>
       <c r="J89">
         <v>86.5</v>
@@ -10365,7 +11824,7 @@
         <v>2.31</v>
       </c>
       <c r="I90">
-        <v>0.69430000000000003</v>
+        <v>-0.69430000000000003</v>
       </c>
       <c r="J90">
         <v>87.5</v>
@@ -10403,7 +11862,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="I91">
-        <v>0.57499999999999996</v>
+        <v>-0.57499999999999996</v>
       </c>
       <c r="J91">
         <v>88.5</v>
@@ -10441,7 +11900,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="I92">
-        <v>0.4536</v>
+        <v>-0.4536</v>
       </c>
       <c r="J92">
         <v>89.5</v>
@@ -10479,7 +11938,7 @@
         <v>2.68</v>
       </c>
       <c r="I93">
-        <v>0.31690000000000002</v>
+        <v>-0.31690000000000002</v>
       </c>
       <c r="J93">
         <v>90.5</v>
@@ -10517,7 +11976,7 @@
         <v>2.81</v>
       </c>
       <c r="I94">
-        <v>0.19239999999999999</v>
+        <v>-0.19239999999999999</v>
       </c>
       <c r="J94">
         <v>91.5</v>
@@ -10555,7 +12014,7 @@
         <v>2.93</v>
       </c>
       <c r="I95">
-        <v>7.0000000000000007E-2</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="J95">
         <v>92.5</v>
@@ -10593,7 +12052,7 @@
         <v>3.03</v>
       </c>
       <c r="I96">
-        <v>-3.3099999999999997E-2</v>
+        <v>3.3099999999999997E-2</v>
       </c>
       <c r="J96">
         <v>93.5</v>
@@ -10631,7 +12090,7 @@
         <v>3.14</v>
       </c>
       <c r="I97">
-        <v>-0.1351</v>
+        <v>0.1351</v>
       </c>
       <c r="J97">
         <v>94.5</v>
@@ -10669,7 +12128,7 @@
         <v>3.2</v>
       </c>
       <c r="I98">
-        <v>-0.1993</v>
+        <v>0.1993</v>
       </c>
       <c r="J98">
         <v>95.5</v>
@@ -10707,7 +12166,7 @@
         <v>3.23</v>
       </c>
       <c r="I99">
-        <v>-0.22889999999999999</v>
+        <v>0.22889999999999999</v>
       </c>
       <c r="J99">
         <v>96.5</v>
@@ -10745,7 +12204,7 @@
         <v>3.23</v>
       </c>
       <c r="I100">
-        <v>-0.23</v>
+        <v>0.23</v>
       </c>
       <c r="J100">
         <v>97.5</v>
@@ -10783,7 +12242,7 @@
         <v>3.23</v>
       </c>
       <c r="I101">
-        <v>-0.22589999999999999</v>
+        <v>0.22589999999999999</v>
       </c>
       <c r="J101">
         <v>98.5</v>
@@ -10821,7 +12280,7 @@
         <v>3.18</v>
       </c>
       <c r="I102">
-        <v>-0.184</v>
+        <v>0.184</v>
       </c>
       <c r="J102">
         <v>99.5</v>
@@ -10859,7 +12318,7 @@
         <v>3.12</v>
       </c>
       <c r="I103">
-        <v>-0.1167</v>
+        <v>0.1167</v>
       </c>
       <c r="J103">
         <v>100.5</v>
@@ -10897,7 +12356,7 @@
         <v>3.06</v>
       </c>
       <c r="I104">
-        <v>-6.1600000000000002E-2</v>
+        <v>6.1600000000000002E-2</v>
       </c>
       <c r="J104">
         <v>101.55</v>
@@ -10935,7 +12394,7 @@
         <v>2.99</v>
       </c>
       <c r="I105">
-        <v>7.7999999999999996E-3</v>
+        <v>-7.7999999999999996E-3</v>
       </c>
       <c r="J105">
         <v>102.55</v>
@@ -10973,7 +12432,7 @@
         <v>2.94</v>
       </c>
       <c r="I106">
-        <v>6.2799999999999995E-2</v>
+        <v>-6.2799999999999995E-2</v>
       </c>
       <c r="J106">
         <v>103.55</v>
@@ -11011,7 +12470,7 @@
         <v>2.94</v>
       </c>
       <c r="I107">
-        <v>6.08E-2</v>
+        <v>-6.08E-2</v>
       </c>
       <c r="J107">
         <v>104.55</v>
@@ -11049,7 +12508,7 @@
         <v>2.98</v>
       </c>
       <c r="I108">
-        <v>2.1999999999999999E-2</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="J108">
         <v>105.55</v>
@@ -11087,7 +12546,7 @@
         <v>3.04</v>
       </c>
       <c r="I109">
-        <v>-4.1200000000000001E-2</v>
+        <v>4.1200000000000001E-2</v>
       </c>
       <c r="J109">
         <v>106.55</v>
@@ -11125,7 +12584,7 @@
         <v>3.11</v>
       </c>
       <c r="I110">
-        <v>-0.1096</v>
+        <v>0.1096</v>
       </c>
       <c r="J110">
         <v>107.55</v>
@@ -11163,7 +12622,7 @@
         <v>3.16</v>
       </c>
       <c r="I111">
-        <v>-0.16159999999999999</v>
+        <v>0.16159999999999999</v>
       </c>
       <c r="J111">
         <v>108.55</v>
@@ -11201,7 +12660,7 @@
         <v>3.19</v>
       </c>
       <c r="I112">
-        <v>-0.18509999999999999</v>
+        <v>0.18509999999999999</v>
       </c>
       <c r="J112">
         <v>109.55</v>
@@ -11239,7 +12698,7 @@
         <v>3.18</v>
       </c>
       <c r="I113">
-        <v>-0.1769</v>
+        <v>0.1769</v>
       </c>
       <c r="J113">
         <v>110.55</v>
@@ -11277,7 +12736,7 @@
         <v>3.14</v>
       </c>
       <c r="I114">
-        <v>-0.14319999999999999</v>
+        <v>0.14319999999999999</v>
       </c>
       <c r="J114">
         <v>111.55</v>
@@ -11315,7 +12774,7 @@
         <v>3.08</v>
       </c>
       <c r="I115">
-        <v>-0.08</v>
+        <v>0.08</v>
       </c>
       <c r="J115">
         <v>112.55</v>
@@ -11353,7 +12812,7 @@
         <v>3.02</v>
       </c>
       <c r="I116">
-        <v>-1.9800000000000002E-2</v>
+        <v>1.9800000000000002E-2</v>
       </c>
       <c r="J116">
         <v>113.55</v>
@@ -11391,7 +12850,7 @@
         <v>2.95</v>
       </c>
       <c r="I117">
-        <v>5.0599999999999999E-2</v>
+        <v>-5.0599999999999999E-2</v>
       </c>
       <c r="J117">
         <v>114.55</v>
@@ -11429,7 +12888,7 @@
         <v>2.91</v>
       </c>
       <c r="I118">
-        <v>9.35E-2</v>
+        <v>-9.35E-2</v>
       </c>
       <c r="J118">
         <v>115.55</v>
@@ -11467,7 +12926,7 @@
         <v>2.9</v>
       </c>
       <c r="I119">
-        <v>9.9599999999999994E-2</v>
+        <v>-9.9599999999999994E-2</v>
       </c>
       <c r="J119">
         <v>116.55</v>
@@ -11505,7 +12964,7 @@
         <v>2.96</v>
       </c>
       <c r="I120">
-        <v>3.6299999999999999E-2</v>
+        <v>-3.6299999999999999E-2</v>
       </c>
       <c r="J120">
         <v>117.6</v>
@@ -11543,7 +13002,7 @@
         <v>3.03</v>
       </c>
       <c r="I121">
-        <v>-2.9000000000000001E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="J121">
         <v>118.6</v>
@@ -11581,7 +13040,7 @@
         <v>3.1</v>
       </c>
       <c r="I122">
-        <v>-9.6299999999999997E-2</v>
+        <v>9.6299999999999997E-2</v>
       </c>
       <c r="J122">
         <v>119.6</v>
@@ -11619,7 +13078,7 @@
         <v>3.16</v>
       </c>
       <c r="I123">
-        <v>0.34250000000000003</v>
+        <v>-0.34250000000000003</v>
       </c>
       <c r="J123">
         <v>120.6</v>
@@ -11657,7 +13116,7 @@
         <v>3.24</v>
       </c>
       <c r="I124">
-        <v>0.26190000000000002</v>
+        <v>-0.26190000000000002</v>
       </c>
       <c r="J124">
         <v>121.6</v>
@@ -11695,7 +13154,7 @@
         <v>3.35</v>
       </c>
       <c r="I125">
-        <v>0.15479999999999999</v>
+        <v>-0.15479999999999999</v>
       </c>
       <c r="J125">
         <v>122.6</v>
@@ -11733,7 +13192,7 @@
         <v>3.47</v>
       </c>
       <c r="I126">
-        <v>2.8299999999999999E-2</v>
+        <v>-2.8299999999999999E-2</v>
       </c>
       <c r="J126">
         <v>123.6</v>
@@ -11771,7 +13230,7 @@
         <v>3.6</v>
       </c>
       <c r="I127">
-        <v>-9.6199999999999994E-2</v>
+        <v>9.6199999999999994E-2</v>
       </c>
       <c r="J127">
         <v>124.6</v>
@@ -11809,7 +13268,7 @@
         <v>3.7</v>
       </c>
       <c r="I128">
-        <v>-0.20230000000000001</v>
+        <v>0.20230000000000001</v>
       </c>
       <c r="J128">
         <v>125.6</v>
@@ -11847,7 +13306,7 @@
         <v>3.77</v>
       </c>
       <c r="I129">
-        <v>-0.2747</v>
+        <v>0.2747</v>
       </c>
       <c r="J129">
         <v>126.65</v>
@@ -11885,7 +13344,7 @@
         <v>3.84</v>
       </c>
       <c r="I130">
-        <v>-0.33600000000000002</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="J130">
         <v>127.65</v>
@@ -11923,7 +13382,7 @@
         <v>3.83</v>
       </c>
       <c r="I131">
-        <v>-0.32879999999999998</v>
+        <v>0.32879999999999998</v>
       </c>
       <c r="J131">
         <v>128.65</v>
@@ -11961,7 +13420,7 @@
         <v>3.83</v>
       </c>
       <c r="I132">
-        <v>-0.32979999999999998</v>
+        <v>0.32979999999999998</v>
       </c>
       <c r="J132">
         <v>129.65</v>
@@ -11999,7 +13458,7 @@
         <v>3.81</v>
       </c>
       <c r="I133">
-        <v>-0.30940000000000001</v>
+        <v>0.30940000000000001</v>
       </c>
       <c r="J133">
         <v>130.65</v>
@@ -12037,7 +13496,7 @@
         <v>3.79</v>
       </c>
       <c r="I134">
-        <v>-0.29409999999999997</v>
+        <v>0.29409999999999997</v>
       </c>
       <c r="J134">
         <v>131.65</v>
@@ -12075,7 +13534,7 @@
         <v>3.76</v>
       </c>
       <c r="I135">
-        <v>-0.26150000000000001</v>
+        <v>0.26150000000000001</v>
       </c>
       <c r="J135">
         <v>132.65</v>
@@ -12113,7 +13572,7 @@
         <v>3.74</v>
       </c>
       <c r="I136">
-        <v>-0.24210000000000001</v>
+        <v>0.24210000000000001</v>
       </c>
       <c r="J136">
         <v>133.65</v>
@@ -12151,7 +13610,7 @@
         <v>3.7</v>
       </c>
       <c r="I137">
-        <v>-0.19719999999999999</v>
+        <v>0.19719999999999999</v>
       </c>
       <c r="J137">
         <v>134.65</v>
@@ -12189,7 +13648,7 @@
         <v>3.67</v>
       </c>
       <c r="I138">
-        <v>-0.16969999999999999</v>
+        <v>0.16969999999999999</v>
       </c>
       <c r="J138">
         <v>135.65</v>
@@ -12227,7 +13686,7 @@
         <v>3.64</v>
       </c>
       <c r="I139">
-        <v>-0.14419999999999999</v>
+        <v>0.14419999999999999</v>
       </c>
       <c r="J139">
         <v>136.65</v>
@@ -12265,7 +13724,7 @@
         <v>3.61</v>
       </c>
       <c r="I140">
-        <v>-0.11459999999999999</v>
+        <v>0.11459999999999999</v>
       </c>
       <c r="J140">
         <v>137.65</v>
@@ -12303,7 +13762,7 @@
         <v>3.57</v>
       </c>
       <c r="I141">
-        <v>-7.2700000000000001E-2</v>
+        <v>7.2700000000000001E-2</v>
       </c>
       <c r="J141">
         <v>138.65</v>
@@ -12341,7 +13800,7 @@
         <v>3.54</v>
       </c>
       <c r="I142">
-        <v>-4.2099999999999999E-2</v>
+        <v>4.2099999999999999E-2</v>
       </c>
       <c r="J142">
         <v>139.65</v>
@@ -12379,7 +13838,7 @@
         <v>3.5</v>
       </c>
       <c r="I143">
-        <v>-4.4000000000000003E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="J143">
         <v>140.65</v>
@@ -12417,7 +13876,7 @@
         <v>3.48</v>
       </c>
       <c r="I144">
-        <v>2.4199999999999999E-2</v>
+        <v>-2.4199999999999999E-2</v>
       </c>
       <c r="J144">
         <v>141.65</v>
@@ -12455,7 +13914,7 @@
         <v>3.46</v>
       </c>
       <c r="I145">
-        <v>4.2500000000000003E-2</v>
+        <v>-4.2500000000000003E-2</v>
       </c>
       <c r="J145">
         <v>142.69999999999999</v>
@@ -12493,7 +13952,7 @@
         <v>3.46</v>
       </c>
       <c r="I146">
-        <v>3.7400000000000003E-2</v>
+        <v>-3.7400000000000003E-2</v>
       </c>
       <c r="J146">
         <v>143.69999999999999</v>
@@ -12531,7 +13990,7 @@
         <v>3.5</v>
       </c>
       <c r="I147">
-        <v>3.8E-3</v>
+        <v>-3.8E-3</v>
       </c>
       <c r="J147">
         <v>144.69999999999999</v>
@@ -12569,7 +14028,7 @@
         <v>3.55</v>
       </c>
       <c r="I148">
-        <v>-1.0523</v>
+        <v>1.0523</v>
       </c>
       <c r="J148">
         <v>145.69999999999999</v>
@@ -12607,7 +14066,7 @@
         <v>3.61</v>
       </c>
       <c r="I149">
-        <v>-1.1073999999999999</v>
+        <v>1.1073999999999999</v>
       </c>
       <c r="J149">
         <v>146.69999999999999</v>
@@ -12645,7 +14104,7 @@
         <v>3.66</v>
       </c>
       <c r="I150">
-        <v>-1.1554</v>
+        <v>1.1554</v>
       </c>
       <c r="J150">
         <v>147.69999999999999</v>
@@ -12683,7 +14142,7 @@
         <v>3.69</v>
       </c>
       <c r="I151">
-        <v>-1.1879999999999999</v>
+        <v>1.1879999999999999</v>
       </c>
       <c r="J151">
         <v>148.69999999999999</v>
@@ -12721,7 +14180,7 @@
         <v>3.7</v>
       </c>
       <c r="I152">
-        <v>-1.2042999999999999</v>
+        <v>1.2042999999999999</v>
       </c>
       <c r="J152">
         <v>149.69999999999999</v>
@@ -12759,7 +14218,7 @@
         <v>3.72</v>
       </c>
       <c r="I153">
-        <v>-1.2185999999999999</v>
+        <v>1.2185999999999999</v>
       </c>
       <c r="J153">
         <v>150.69999999999999</v>
@@ -12797,7 +14256,7 @@
         <v>3.71</v>
       </c>
       <c r="I154">
-        <v>-1.2144999999999999</v>
+        <v>1.2144999999999999</v>
       </c>
       <c r="J154">
         <v>151.69999999999999</v>
@@ -12835,7 +14294,7 @@
         <v>3.71</v>
       </c>
       <c r="I155">
-        <v>-1.2124999999999999</v>
+        <v>1.2124999999999999</v>
       </c>
       <c r="J155">
         <v>152.69999999999999</v>
@@ -12873,7 +14332,7 @@
         <v>3.7</v>
       </c>
       <c r="I156">
-        <v>-1.2022999999999999</v>
+        <v>1.2022999999999999</v>
       </c>
       <c r="J156">
         <v>153.69999999999999</v>
@@ -12911,7 +14370,7 @@
         <v>3.68</v>
       </c>
       <c r="I157">
-        <v>-1.1850000000000001</v>
+        <v>1.1850000000000001</v>
       </c>
       <c r="J157">
         <v>154.69999999999999</v>
@@ -12949,7 +14408,7 @@
         <v>3.66</v>
       </c>
       <c r="I158">
-        <v>-1.1625000000000001</v>
+        <v>1.1625000000000001</v>
       </c>
       <c r="J158">
         <v>155.69999999999999</v>
@@ -12987,7 +14446,7 @@
         <v>3.64</v>
       </c>
       <c r="I159">
-        <v>-1.1391</v>
+        <v>1.1391</v>
       </c>
       <c r="J159">
         <v>156.69999999999999</v>
@@ -13025,7 +14484,7 @@
         <v>3.61</v>
       </c>
       <c r="I160">
-        <v>-1.1053999999999999</v>
+        <v>1.1053999999999999</v>
       </c>
       <c r="J160">
         <v>157.71</v>
@@ -13063,7 +14522,7 @@
         <v>3.58</v>
       </c>
       <c r="I161">
-        <v>-1.0809</v>
+        <v>1.0809</v>
       </c>
       <c r="J161">
         <v>158.76</v>
@@ -13101,7 +14560,7 @@
         <v>3.54</v>
       </c>
       <c r="I162">
-        <v>-1.0421</v>
+        <v>1.0421</v>
       </c>
       <c r="J162">
         <v>159.76</v>
@@ -13139,7 +14598,7 @@
         <v>3.51</v>
       </c>
       <c r="I163">
-        <v>-1.0054000000000001</v>
+        <v>1.0054000000000001</v>
       </c>
       <c r="J163">
         <v>160.76</v>
@@ -13177,7 +14636,7 @@
         <v>3.47</v>
       </c>
       <c r="I164">
-        <v>-0.9738</v>
+        <v>0.9738</v>
       </c>
       <c r="J164">
         <v>161.76</v>
@@ -13215,7 +14674,7 @@
         <v>3.43</v>
       </c>
       <c r="I165">
-        <v>-0.92579999999999996</v>
+        <v>0.92579999999999996</v>
       </c>
       <c r="J165">
         <v>162.76</v>
@@ -13253,7 +14712,7 @@
         <v>3.38</v>
       </c>
       <c r="I166">
-        <v>-0.88400000000000001</v>
+        <v>0.88400000000000001</v>
       </c>
       <c r="J166">
         <v>163.76</v>
@@ -13291,7 +14750,7 @@
         <v>3.35</v>
       </c>
       <c r="I167">
-        <v>-0.84630000000000005</v>
+        <v>0.84630000000000005</v>
       </c>
       <c r="J167">
         <v>164.76</v>
@@ -13329,7 +14788,7 @@
         <v>3.3</v>
       </c>
       <c r="I168">
-        <v>-0.79930000000000001</v>
+        <v>0.79930000000000001</v>
       </c>
       <c r="J168">
         <v>165.76</v>
@@ -13367,7 +14826,7 @@
         <v>3.25</v>
       </c>
       <c r="I169">
-        <v>-0.74929999999999997</v>
+        <v>0.74929999999999997</v>
       </c>
       <c r="J169">
         <v>166.76</v>
@@ -13405,7 +14864,7 @@
         <v>3.2</v>
       </c>
       <c r="I170">
-        <v>-0.70240000000000002</v>
+        <v>0.70240000000000002</v>
       </c>
       <c r="J170">
         <v>167.81</v>
@@ -13443,7 +14902,7 @@
         <v>3.15</v>
       </c>
       <c r="I171">
-        <v>-0.64529999999999998</v>
+        <v>0.64529999999999998</v>
       </c>
       <c r="J171">
         <v>168.81</v>
@@ -13481,7 +14940,7 @@
         <v>3.1</v>
       </c>
       <c r="I172">
-        <v>-0.59530000000000005</v>
+        <v>0.59530000000000005</v>
       </c>
       <c r="J172">
         <v>169.81</v>
@@ -13519,7 +14978,7 @@
         <v>3.05</v>
       </c>
       <c r="I173">
-        <v>-0.54530000000000001</v>
+        <v>0.54530000000000001</v>
       </c>
       <c r="J173">
         <v>170.81</v>
@@ -13557,7 +15016,7 @@
         <v>2.99</v>
       </c>
       <c r="I174">
-        <v>-0.48509999999999998</v>
+        <v>0.48509999999999998</v>
       </c>
       <c r="J174">
         <v>171.81</v>
@@ -13595,7 +15054,7 @@
         <v>2.93</v>
       </c>
       <c r="I175">
-        <v>-0.43309999999999998</v>
+        <v>0.43309999999999998</v>
       </c>
       <c r="J175">
         <v>172.81</v>
@@ -13633,7 +15092,7 @@
         <v>2.89</v>
       </c>
       <c r="I176">
-        <v>-0.3861</v>
+        <v>0.3861</v>
       </c>
       <c r="J176">
         <v>173.81</v>
@@ -13671,7 +15130,7 @@
         <v>2.83</v>
       </c>
       <c r="I177">
-        <v>-0.32600000000000001</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="J177">
         <v>174.81</v>
@@ -13709,7 +15168,7 @@
         <v>2.76</v>
       </c>
       <c r="I178">
-        <v>-0.26369999999999999</v>
+        <v>0.26369999999999999</v>
       </c>
       <c r="J178">
         <v>175.81</v>
@@ -13747,7 +15206,7 @@
         <v>2.71</v>
       </c>
       <c r="I179">
-        <v>-0.2097</v>
+        <v>0.2097</v>
       </c>
       <c r="J179">
         <v>176.81</v>
@@ -13785,7 +15244,7 @@
         <v>2.64</v>
       </c>
       <c r="I180">
-        <v>-0.13819999999999999</v>
+        <v>0.13819999999999999</v>
       </c>
       <c r="J180">
         <v>177.81</v>
@@ -13823,7 +15282,7 @@
         <v>2.58</v>
       </c>
       <c r="I181">
-        <v>-7.6999999999999999E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="J181">
         <v>178.81</v>
@@ -13861,7 +15320,7 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="I182">
-        <v>-1.4800000000000001E-2</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="J182">
         <v>179.81</v>
@@ -13899,7 +15358,7 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="I183">
-        <v>5.1499999999999997E-2</v>
+        <v>-5.1499999999999997E-2</v>
       </c>
       <c r="J183">
         <v>180.81</v>
@@ -13937,7 +15396,7 @@
         <v>2.38</v>
       </c>
       <c r="I184">
-        <v>0.1178</v>
+        <v>-0.1178</v>
       </c>
       <c r="J184">
         <v>181.81</v>
@@ -13975,7 +15434,7 @@
         <v>2.33</v>
       </c>
       <c r="I185">
-        <v>0.1709</v>
+        <v>-0.1709</v>
       </c>
       <c r="J185">
         <v>182.81</v>
@@ -14013,7 +15472,7 @@
         <v>2.31</v>
       </c>
       <c r="I186">
-        <v>0.18820000000000001</v>
+        <v>-0.18820000000000001</v>
       </c>
       <c r="J186">
         <v>183.81</v>
@@ -14051,7 +15510,7 @@
         <v>2.36</v>
       </c>
       <c r="I187">
-        <v>0.13819999999999999</v>
+        <v>-0.13819999999999999</v>
       </c>
       <c r="J187">
         <v>184.86</v>
@@ -14089,7 +15548,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="I188">
-        <v>7.2900000000000006E-2</v>
+        <v>-7.2900000000000006E-2</v>
       </c>
       <c r="J188">
         <v>185.86</v>
@@ -14127,7 +15586,7 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="I189">
-        <v>-1.17E-2</v>
+        <v>1.17E-2</v>
       </c>
       <c r="J189">
         <v>186.86</v>
@@ -14165,7 +15624,7 @@
         <v>2.59</v>
       </c>
       <c r="I190">
-        <v>-8.72E-2</v>
+        <v>8.72E-2</v>
       </c>
       <c r="J190">
         <v>187.86</v>
@@ -14203,7 +15662,7 @@
         <v>2.64</v>
       </c>
       <c r="I191">
-        <v>-0.13819999999999999</v>
+        <v>0.13819999999999999</v>
       </c>
       <c r="J191">
         <v>188.86</v>
@@ -14241,7 +15700,7 @@
         <v>2.66</v>
       </c>
       <c r="I192">
-        <v>-0.16070000000000001</v>
+        <v>0.16070000000000001</v>
       </c>
       <c r="J192">
         <v>189.86</v>
@@ -14279,7 +15738,7 @@
         <v>2.65</v>
       </c>
       <c r="I193">
-        <v>-0.1515</v>
+        <v>0.1515</v>
       </c>
       <c r="J193">
         <v>190.86</v>
@@ -14317,7 +15776,7 @@
         <v>2.61</v>
       </c>
       <c r="I194">
-        <v>-0.1138</v>
+        <v>0.1138</v>
       </c>
       <c r="J194">
         <v>191.86</v>
@@ -14355,7 +15814,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="I195">
-        <v>-4.7399999999999998E-2</v>
+        <v>4.7399999999999998E-2</v>
       </c>
       <c r="J195">
         <v>192.86</v>
@@ -14393,7 +15852,7 @@
         <v>2.4700000000000002</v>
       </c>
       <c r="I196">
-        <v>3.0099999999999998E-2</v>
+        <v>-3.0099999999999998E-2</v>
       </c>
       <c r="J196">
         <v>193.86</v>
@@ -14431,7 +15890,7 @@
         <v>2.4</v>
       </c>
       <c r="I197">
-        <v>0.10150000000000001</v>
+        <v>-0.10150000000000001</v>
       </c>
       <c r="J197">
         <v>194.86</v>
@@ -14469,7 +15928,7 @@
         <v>2.38</v>
       </c>
       <c r="I198">
-        <v>0.125</v>
+        <v>-0.125</v>
       </c>
       <c r="J198">
         <v>195.86</v>
@@ -14507,7 +15966,7 @@
         <v>2.4</v>
       </c>
       <c r="I199">
-        <v>0.1046</v>
+        <v>-0.1046</v>
       </c>
       <c r="J199">
         <v>196.86</v>
@@ -14545,7 +16004,7 @@
         <v>2.44</v>
       </c>
       <c r="I200">
-        <v>5.6599999999999998E-2</v>
+        <v>-5.6599999999999998E-2</v>
       </c>
       <c r="J200">
         <v>197.86</v>
@@ -14583,7 +16042,7 @@
         <v>2.52</v>
       </c>
       <c r="I201">
-        <v>-2.3E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="J201">
         <v>198.86</v>
@@ -14621,7 +16080,7 @@
         <v>2.6</v>
       </c>
       <c r="I202">
-        <v>-9.8400000000000001E-2</v>
+        <v>9.8400000000000001E-2</v>
       </c>
       <c r="J202">
         <v>199.91</v>
@@ -14659,7 +16118,7 @@
         <v>2.65</v>
       </c>
       <c r="I203">
-        <v>-0.1474</v>
+        <v>0.1474</v>
       </c>
       <c r="J203">
         <v>200.91</v>
@@ -14697,7 +16156,7 @@
         <v>2.67</v>
       </c>
       <c r="I204">
-        <v>-0.1699</v>
+        <v>0.1699</v>
       </c>
       <c r="J204">
         <v>201.91</v>
@@ -14735,7 +16194,7 @@
         <v>2.65</v>
       </c>
       <c r="I205">
-        <v>-0.1484</v>
+        <v>0.1484</v>
       </c>
       <c r="J205">
         <v>202.91</v>
@@ -14773,7 +16232,7 @@
         <v>2.61</v>
       </c>
       <c r="I206">
-        <v>-0.1138</v>
+        <v>0.1138</v>
       </c>
       <c r="J206">
         <v>203.91</v>
@@ -14811,7 +16270,7 @@
         <v>2.54</v>
       </c>
       <c r="I207">
-        <v>-4.1300000000000003E-2</v>
+        <v>4.1300000000000003E-2</v>
       </c>
       <c r="J207">
         <v>204.91</v>
@@ -14849,7 +16308,7 @@
         <v>2.46</v>
       </c>
       <c r="I208">
-        <v>-2.4607000000000001</v>
+        <v>2.4607000000000001</v>
       </c>
       <c r="J208">
         <v>205.11</v>
@@ -14887,7 +16346,7 @@
         <v>2.36</v>
       </c>
       <c r="I209">
-        <v>-2.3607</v>
+        <v>2.3607</v>
       </c>
       <c r="J209">
         <v>205.11</v>
@@ -14925,7 +16384,7 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="I210">
-        <v>-2.2566999999999999</v>
+        <v>2.2566999999999999</v>
       </c>
       <c r="J210">
         <v>205.11</v>
@@ -14963,7 +16422,7 @@
         <v>2.15</v>
       </c>
       <c r="I211">
-        <v>-2.1475</v>
+        <v>2.1475</v>
       </c>
       <c r="J211">
         <v>205.11</v>
@@ -15001,7 +16460,7 @@
         <v>2.04</v>
       </c>
       <c r="I212">
-        <v>-2.0434999999999999</v>
+        <v>2.0434999999999999</v>
       </c>
       <c r="J212">
         <v>205.11</v>
@@ -15039,7 +16498,7 @@
         <v>1.93</v>
       </c>
       <c r="I213">
-        <v>-1.9322999999999999</v>
+        <v>1.9322999999999999</v>
       </c>
       <c r="J213">
         <v>205.11</v>
@@ -15077,7 +16536,7 @@
         <v>1.83</v>
       </c>
       <c r="I214">
-        <v>-1.8262</v>
+        <v>1.8262</v>
       </c>
       <c r="J214">
         <v>205.11</v>
@@ -15115,7 +16574,7 @@
         <v>1.73</v>
       </c>
       <c r="I215">
-        <v>-1.7262</v>
+        <v>1.7262</v>
       </c>
       <c r="J215">
         <v>205.11</v>
@@ -15153,7 +16612,7 @@
         <v>1.62</v>
       </c>
       <c r="I216">
-        <v>-1.6242000000000001</v>
+        <v>1.6242000000000001</v>
       </c>
       <c r="J216">
         <v>205.11</v>
@@ -15191,7 +16650,7 @@
         <v>1.53</v>
       </c>
       <c r="I217">
-        <v>-1.5344</v>
+        <v>1.5344</v>
       </c>
       <c r="J217">
         <v>205.11</v>
@@ -15229,7 +16688,7 @@
         <v>1.43</v>
       </c>
       <c r="I218">
-        <v>-1.4323999999999999</v>
+        <v>1.4323999999999999</v>
       </c>
       <c r="J218">
         <v>205.11</v>
@@ -15267,7 +16726,7 @@
         <v>1.33</v>
       </c>
       <c r="I219">
-        <v>-1.3324</v>
+        <v>1.3324</v>
       </c>
       <c r="J219">
         <v>205.11</v>
@@ -15305,7 +16764,7 @@
         <v>1.22</v>
       </c>
       <c r="I220">
-        <v>-1.2181</v>
+        <v>1.2181</v>
       </c>
       <c r="J220">
         <v>205.11</v>
@@ -15343,7 +16802,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="I221">
-        <v>-1.1212</v>
+        <v>1.1212</v>
       </c>
       <c r="J221">
         <v>205.11</v>
@@ -15381,7 +16840,7 @@
         <v>1.01</v>
       </c>
       <c r="I222">
-        <v>-1.0109999999999999</v>
+        <v>1.0109999999999999</v>
       </c>
       <c r="J222">
         <v>205.11</v>
@@ -15419,7 +16878,7 @@
         <v>0.9</v>
       </c>
       <c r="I223">
-        <v>-0.89980000000000004</v>
+        <v>0.89980000000000004</v>
       </c>
       <c r="J223">
         <v>205.11</v>
@@ -15457,7 +16916,7 @@
         <v>0.8</v>
       </c>
       <c r="I224">
-        <v>-0.79579999999999995</v>
+        <v>0.79579999999999995</v>
       </c>
       <c r="J224">
         <v>205.11</v>
@@ -15495,7 +16954,7 @@
         <v>0.68</v>
       </c>
       <c r="I225">
-        <v>-0.6764</v>
+        <v>0.6764</v>
       </c>
       <c r="J225">
         <v>205.11</v>
@@ -15533,7 +16992,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="I226">
-        <v>-0.57230000000000003</v>
+        <v>0.57230000000000003</v>
       </c>
       <c r="J226">
         <v>205.11</v>
@@ -15571,7 +17030,7 @@
         <v>0.45</v>
       </c>
       <c r="I227">
-        <v>-0.44579999999999997</v>
+        <v>0.44579999999999997</v>
       </c>
       <c r="J227">
         <v>205.11</v>

</xml_diff>